<commit_message>
Remove Test cases for SD and mean
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 10/Iteration 10 Test Cases.xlsx
+++ b/Test Cases/Iteration 10/Iteration 10 Test Cases.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="360">
   <si>
     <t>No</t>
   </si>
@@ -3216,104 +3216,6 @@
   <si>
     <t>Team: Visa
 Date: 2016-07-01 to 2016-07-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index (S.D &amp; Mean) </t>
-  </si>
-  <si>
-    <t>Team: Medical / VISA
-Date:  2016-06-31 To 2016-01-01</t>
-  </si>
-  <si>
-    <t>Team: Medical / VISA
-Date: 2016-01-01 to 2016-06-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical Score  : Count / % 
-0    :   142   / 91.6%
-1    :   10   / 6.45%
-2    :   3  / 1.9%
-3    :   0 / 0%
-Total : 155
-SD:  0.5547  
-Mean: 0.103 
-Team Score  : Count / % 
-0    :    25   / 53.2%
-1    :   7  / 14.9%
-2    :   12  /  25.5%
-3    :   3 / 6.4% 
-Total : 47 
-SD: 0.639
-Mean : 0.85
-</t>
-  </si>
-  <si>
-    <t>Team: Medical / VISA
-Date: 2016-07-01 to 2016-07-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medical Score  : Count / % 
-0    :   18  / 90%
-1    :   2   /  10%
-2    :   0  /  0%
-3    :   0 / 0%
-Total : 20
-SD: 0.307
-Mean: 0.1
-VISA Score  : Count / % 
-0    :   3  / 75%
-1    :   0   /  0%
-2    :   1  /  25%
-3    :   0 / 0%
-Total : 4
-SD: 1 
-Mean: 0.5 </t>
-  </si>
-  <si>
-    <t>Team: Person in charge 
-Date:  2016-06-31 To 2016-01-01</t>
-  </si>
-  <si>
-    <t>Team: Person in charge
-Date: 2016-01-01 to 2016-06-31</t>
-  </si>
-  <si>
-    <t>Andreas Score / Count 
-0 : 31
-Jeslyn Score / Count 
-0 : 20
-1 : 1 
-Sanjit Score / Count 
-0 : 49   
-1 : 7 
-2 : 1  
-Zin  Score / Count 
-0 : 35   
-1 : 1 
-2 : 1 
-No Followup Person Score / Count 
-0 : 35
-1 : 8
-2 : 11 
-3 : 2    
-Total : 56</t>
-  </si>
-  <si>
-    <t>Team: Person in charge
-Date: 2016-07-01 to 2016-07-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andreas  Score / Count 
-0 : 1
-Sanjit Score / Count 
-0 : 7   
-1 : 1 
-Zin  Score / Count 
-0 : 4   
-No Followup Person 
-0 :  9 
-1 : 1
-2 : 1 </t>
   </si>
   <si>
     <r>
@@ -6920,10 +6822,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7035,7 +6937,7 @@
         <v>355</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="154" x14ac:dyDescent="0.35">
@@ -7049,92 +6951,44 @@
         <v>357</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A9" s="28">
-        <v>7</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="C9" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="D9" s="28" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="279" x14ac:dyDescent="0.35">
-      <c r="A10" s="28">
-        <v>8</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="263.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="28">
-        <v>9</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>362</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A12" s="28">
-        <v>10</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>364</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="372" x14ac:dyDescent="0.35">
-      <c r="A13" s="28">
-        <v>11</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>365</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="217" x14ac:dyDescent="0.35">
-      <c r="A14" s="28">
-        <v>12</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>367</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>368</v>
-      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="28"/>
@@ -7165,42 +7019,6 @@
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7356,7 +7174,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="263.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="248" x14ac:dyDescent="0.35">
       <c r="A10" s="28">
         <v>8</v>
       </c>
@@ -7440,7 +7258,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="155" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A16" s="28">
         <v>14</v>
       </c>
@@ -7468,7 +7286,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="28">
         <v>16</v>
       </c>

</xml_diff>